<commit_message>
Finalizando os scripts DQL
</commit_message>
<xml_diff>
--- a/SENAI-Sprint.1-BD/Desafio - RPG/Modelo-Fisico.xlsx
+++ b/SENAI-Sprint.1-BD/Desafio - RPG/Modelo-Fisico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flávia\Documents\Python Scripts\Técnico\Segundo semestre\SENAI-Segundo.Semestre\SENAI-Sprint.1-BD\Desafio - RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793A2DFC-78E9-44D5-8AAA-5B80D8C20768}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4907FE-46F6-4A7D-8100-6390B46D210C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CD7F21A-A962-4162-B510-12B87DE775D2}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{8CD7F21A-A962-4162-B510-12B87DE775D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
-    <t>Personagem</t>
-  </si>
-  <si>
     <t>idPersonagem</t>
   </si>
   <si>
@@ -114,13 +111,16 @@
     <t>idHabilidade</t>
   </si>
   <si>
-    <t>ClasseHabilidades</t>
-  </si>
-  <si>
     <t>BitBug</t>
   </si>
   <si>
     <t>Fer8</t>
+  </si>
+  <si>
+    <t>Personagens</t>
+  </si>
+  <si>
+    <t>ClasseHabilidade</t>
   </si>
 </sst>
 </file>
@@ -269,40 +269,40 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -632,7 +632,7 @@
   <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,37 +646,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>8</v>
+      <c r="H3" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>100</v>
@@ -692,10 +692,10 @@
       <c r="E4" s="1">
         <v>80</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="12">
         <v>44256</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="12">
         <v>43483</v>
       </c>
       <c r="H4" s="1">
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1">
         <v>70</v>
@@ -715,11 +715,11 @@
       <c r="E5" s="1">
         <v>100</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="12">
         <f>$F$4</f>
         <v>44256</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="12">
         <v>42446</v>
       </c>
       <c r="H5" s="1">
@@ -731,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1">
         <v>75</v>
@@ -739,11 +739,11 @@
       <c r="E6" s="1">
         <v>60</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="12">
         <f>$F$4</f>
         <v>44256</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="12">
         <v>43542</v>
       </c>
       <c r="H6" s="1">
@@ -751,220 +751,220 @@
       </c>
     </row>
     <row r="9" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7"/>
+      <c r="B9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="D9"/>
-      <c r="F9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="9"/>
+      <c r="F9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10"/>
       <c r="F10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="12">
-        <v>1</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="F12" s="8">
+        <v>2</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="11">
-        <v>2</v>
-      </c>
-      <c r="C12" s="11" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="12">
-        <v>2</v>
-      </c>
-      <c r="G12" s="12" t="s">
+      <c r="F13" s="8">
+        <v>3</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="11">
-        <v>3</v>
-      </c>
-      <c r="C13" s="11" t="s">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="12">
-        <v>3</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="F14" s="8">
+        <v>4</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="11">
-        <v>4</v>
-      </c>
-      <c r="C14" s="11" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="12">
-        <v>4</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
-        <v>5</v>
-      </c>
-      <c r="C15" s="11" t="s">
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="11">
-        <v>6</v>
-      </c>
-      <c r="C16" s="11" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="11">
-        <v>7</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="20" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="B20" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
       <c r="E20"/>
-      <c r="F20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="14"/>
+      <c r="F20" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="F21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11">
+        <v>1</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="9">
         <v>2</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="13">
-        <v>1</v>
-      </c>
-      <c r="C22" s="13" t="s">
+      <c r="C23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="13">
-        <v>1</v>
-      </c>
-      <c r="F22" s="16">
-        <v>1</v>
-      </c>
-      <c r="G22" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
+      <c r="D23" s="9">
         <v>2</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="F23" s="11">
+        <v>1</v>
+      </c>
+      <c r="G23" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="9">
+        <v>3</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D24" s="9">
+        <v>3</v>
+      </c>
+      <c r="F24" s="11">
         <v>2</v>
       </c>
-      <c r="F23" s="16">
-        <v>1</v>
-      </c>
-      <c r="G23" s="16">
+      <c r="G24" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="11">
         <v>3</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="13">
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="11">
+        <v>4</v>
+      </c>
+      <c r="G26" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="11">
+        <v>4</v>
+      </c>
+      <c r="G27" s="11">
         <v>3</v>
       </c>
-      <c r="F24" s="16">
-        <v>2</v>
-      </c>
-      <c r="G24" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F25" s="16">
-        <v>3</v>
-      </c>
-      <c r="G25" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F26" s="16">
-        <v>4</v>
-      </c>
-      <c r="G26" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="16">
-        <v>4</v>
-      </c>
-      <c r="G27" s="16">
-        <v>3</v>
-      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="16">
+      <c r="F28" s="11">
         <v>6</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="11">
         <v>3</v>
       </c>
     </row>

</xml_diff>